<commit_message>
Agrego switch de fibra y Modem Router (imágenes, consumo y presupuesto)
</commit_message>
<xml_diff>
--- a/PRESUPUESTO Y EJEMPLO/PRESUPUESTO.xlsx
+++ b/PRESUPUESTO Y EJEMPLO/PRESUPUESTO.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,12 +11,12 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="46">
   <si>
     <t>Piso:</t>
   </si>
@@ -148,6 +148,12 @@
   </si>
   <si>
     <t>Precio por boca</t>
+  </si>
+  <si>
+    <t>Modem Router</t>
+  </si>
+  <si>
+    <t>Switch Fibra</t>
   </si>
 </sst>
 </file>
@@ -656,10 +662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:L75"/>
+  <dimension ref="A2:L76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N65" sqref="N65"/>
+      <selection activeCell="I64" sqref="I64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -998,17 +1004,17 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="C15" s="5">
         <v>1</v>
       </c>
       <c r="D15" s="10">
-        <v>1700</v>
+        <v>125</v>
       </c>
       <c r="E15" s="10">
         <f>D15*C15</f>
-        <v>1700</v>
+        <v>125</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>6</v>
@@ -1026,18 +1032,17 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="C16" s="5">
-        <f>2*C14+2*C15+2*C19</f>
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="D16" s="10">
-        <v>0.5</v>
+        <v>4120</v>
       </c>
       <c r="E16" s="10">
         <f>D16*C16</f>
-        <v>12</v>
+        <v>4120</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>20</v>
@@ -1056,15 +1061,17 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="19"/>
+        <v>6</v>
+      </c>
+      <c r="C17" s="5">
+        <v>1</v>
+      </c>
       <c r="D17" s="10">
-        <v>0.85</v>
+        <v>1700</v>
       </c>
       <c r="E17" s="10">
-        <f t="shared" ref="E17:E23" si="4">D17*C17</f>
-        <v>0</v>
+        <f>D17*C17</f>
+        <v>1700</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>23</v>
@@ -1074,80 +1081,79 @@
         <v>0.85</v>
       </c>
       <c r="K17" s="10">
-        <f t="shared" ref="K17:K20" si="5">J17*I17</f>
+        <f t="shared" ref="K17:K20" si="4">J17*I17</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="5">
+        <f>2*C14+2*C17+2*C21</f>
+        <v>24</v>
+      </c>
+      <c r="D18" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="E18" s="10">
+        <f>D18*C18</f>
+        <v>12</v>
+      </c>
+      <c r="H18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="10">
-        <v>1</v>
-      </c>
-      <c r="D18" s="10">
+      <c r="I18" s="10">
+        <v>1</v>
+      </c>
+      <c r="J18" s="10">
         <v>1190</v>
       </c>
-      <c r="E18" s="10">
+      <c r="K18" s="10">
         <f t="shared" si="4"/>
         <v>1190</v>
       </c>
-      <c r="H18" s="1" t="s">
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="19"/>
+      <c r="D19" s="10">
+        <v>0.85</v>
+      </c>
+      <c r="E19" s="10">
+        <f t="shared" ref="E19:E25" si="5">D19*C19</f>
+        <v>0</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I19" s="25">
+        <v>6</v>
+      </c>
+      <c r="J19" s="26">
+        <v>12</v>
+      </c>
+      <c r="K19" s="26">
+        <f t="shared" si="4"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I18" s="10">
-        <v>1</v>
-      </c>
-      <c r="J18" s="10">
+      <c r="C20" s="10">
+        <v>1</v>
+      </c>
+      <c r="D20" s="10">
         <v>1190</v>
       </c>
-      <c r="K18" s="10">
+      <c r="E20" s="10">
         <f t="shared" si="5"/>
         <v>1190</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="25">
-        <v>1</v>
-      </c>
-      <c r="D19" s="26">
-        <v>195</v>
-      </c>
-      <c r="E19" s="26">
-        <f t="shared" si="4"/>
-        <v>195</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I19" s="25">
-        <v>6</v>
-      </c>
-      <c r="J19" s="26">
-        <v>12</v>
-      </c>
-      <c r="K19" s="26">
-        <f t="shared" si="5"/>
-        <v>72</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B20" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20" s="25">
-        <v>4</v>
-      </c>
-      <c r="D20" s="26">
-        <v>2499</v>
-      </c>
-      <c r="E20" s="26">
-        <f t="shared" si="4"/>
-        <v>9996</v>
-      </c>
       <c r="H20" s="1" t="s">
         <v>40</v>
       </c>
@@ -1158,964 +1164,994 @@
         <v>13</v>
       </c>
       <c r="K20" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>819</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="C21" s="25">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D21" s="26">
-        <v>12</v>
+        <v>195</v>
       </c>
       <c r="E21" s="26">
-        <f t="shared" si="4"/>
-        <v>36</v>
+        <f t="shared" si="5"/>
+        <v>195</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" s="10">
         <v>30</v>
       </c>
+      <c r="C22" s="25">
+        <v>4</v>
+      </c>
       <c r="D22" s="26">
-        <v>13</v>
+        <v>2499</v>
       </c>
       <c r="E22" s="26">
-        <f t="shared" si="4"/>
-        <v>390</v>
+        <f t="shared" si="5"/>
+        <v>9996</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="25">
+        <v>3</v>
+      </c>
+      <c r="D23" s="26">
+        <v>12</v>
+      </c>
+      <c r="E23" s="26">
+        <f t="shared" si="5"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="10">
+        <v>30</v>
+      </c>
+      <c r="D24" s="26">
+        <v>13</v>
+      </c>
+      <c r="E24" s="26">
+        <f t="shared" si="5"/>
+        <v>390</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="25">
-        <v>1</v>
-      </c>
-      <c r="D23" s="10">
+      <c r="C25" s="25">
+        <v>1</v>
+      </c>
+      <c r="D25" s="10">
         <v>5700</v>
       </c>
-      <c r="E23" s="10">
-        <f t="shared" si="4"/>
+      <c r="E25" s="10">
+        <f t="shared" si="5"/>
         <v>5700</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B26" s="2">
-        <v>2</v>
-      </c>
-      <c r="C26" s="8"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="G26" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H26" s="2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="2">
+        <v>2</v>
+      </c>
+      <c r="C27" s="8"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="G27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H27" s="2">
         <v>3</v>
       </c>
-      <c r="I26" s="8"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="6"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B27" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I27" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="J27" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="K27" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="L27">
-        <v>20</v>
-      </c>
+      <c r="I27" s="8"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C28" s="5">
-        <v>6</v>
-      </c>
-      <c r="D28" s="10">
-        <v>450</v>
-      </c>
-      <c r="E28" s="10">
-        <f>D28*C28</f>
-        <v>2700</v>
+        <v>2</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>8</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I28" s="5">
-        <v>2</v>
-      </c>
-      <c r="J28" s="10">
-        <v>450</v>
-      </c>
-      <c r="K28" s="10">
-        <f>J28*I28</f>
-        <v>900</v>
+        <v>2</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J28" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="K28" s="9" t="s">
+        <v>8</v>
       </c>
       <c r="L28">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C29" s="5">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D29" s="10">
-        <v>1699</v>
+        <v>450</v>
       </c>
       <c r="E29" s="10">
-        <f t="shared" ref="E29" si="6">D29*C29</f>
-        <v>23786</v>
+        <f>D29*C29</f>
+        <v>2700</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I29" s="5">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="J29" s="10">
-        <v>1699</v>
+        <v>450</v>
       </c>
       <c r="K29" s="10">
-        <f t="shared" ref="K29" si="7">J29*I29</f>
-        <v>35679</v>
+        <f>J29*I29</f>
+        <v>900</v>
+      </c>
+      <c r="L29">
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C30" s="5">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="D30" s="10">
-        <v>1700</v>
+        <v>1699</v>
       </c>
       <c r="E30" s="10">
-        <f>D30*C30</f>
-        <v>1700</v>
+        <f t="shared" ref="E30" si="6">D30*C30</f>
+        <v>23786</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I30" s="5">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="J30" s="10">
-        <v>1700</v>
+        <v>1699</v>
       </c>
       <c r="K30" s="10">
-        <f>J30*I30</f>
-        <v>1700</v>
+        <f t="shared" ref="K30" si="7">J30*I30</f>
+        <v>35679</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C31" s="5">
-        <f>2*C29+2*C30</f>
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="D31" s="10">
-        <v>0.5</v>
+        <v>1700</v>
       </c>
       <c r="E31" s="10">
         <f>D31*C31</f>
-        <v>15</v>
+        <v>1700</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="I31" s="5">
-        <f>2*I29+2*I30</f>
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="J31" s="10">
-        <v>0.5</v>
+        <v>1700</v>
       </c>
       <c r="K31" s="10">
         <f>J31*I31</f>
-        <v>22</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C32" s="19"/>
+        <v>20</v>
+      </c>
+      <c r="C32" s="5">
+        <f>2*C30+2*C31</f>
+        <v>30</v>
+      </c>
       <c r="D32" s="10">
-        <v>0.85</v>
+        <v>0.5</v>
       </c>
       <c r="E32" s="10">
-        <f t="shared" ref="E32:E35" si="8">D32*C32</f>
-        <v>0</v>
+        <f>D32*C32</f>
+        <v>15</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I32" s="10"/>
+        <v>20</v>
+      </c>
+      <c r="I32" s="5">
+        <f>2*I30+2*I31</f>
+        <v>44</v>
+      </c>
       <c r="J32" s="10">
-        <v>0.85</v>
+        <v>0.5</v>
       </c>
       <c r="K32" s="10">
-        <f t="shared" ref="K32:K36" si="9">J32*I32</f>
-        <v>0</v>
+        <f>J32*I32</f>
+        <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C33" s="19"/>
+      <c r="D33" s="10">
+        <v>0.85</v>
+      </c>
+      <c r="E33" s="10">
+        <f t="shared" ref="E33:E36" si="8">D33*C33</f>
+        <v>0</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10">
+        <v>0.85</v>
+      </c>
+      <c r="K33" s="10">
+        <f t="shared" ref="K33:K37" si="9">J33*I33</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B34" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C33" s="10">
-        <v>1</v>
-      </c>
-      <c r="D33" s="10">
+      <c r="C34" s="10">
+        <v>1</v>
+      </c>
+      <c r="D34" s="10">
         <v>1190</v>
       </c>
-      <c r="E33" s="10">
+      <c r="E34" s="10">
         <f t="shared" si="8"/>
         <v>1190</v>
       </c>
-      <c r="H33" s="1" t="s">
+      <c r="H34" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I33" s="10">
-        <v>1</v>
-      </c>
-      <c r="J33" s="10">
+      <c r="I34" s="10">
+        <v>1</v>
+      </c>
+      <c r="J34" s="10">
         <v>1190</v>
       </c>
-      <c r="K33" s="10">
+      <c r="K34" s="10">
         <f t="shared" si="9"/>
         <v>1190</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B34" s="1" t="s">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B35" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C34" s="10">
+      <c r="C35" s="10">
         <v>4</v>
       </c>
-      <c r="D34" s="26">
+      <c r="D35" s="26">
         <v>12</v>
       </c>
-      <c r="E34" s="10">
+      <c r="E35" s="10">
         <f t="shared" si="8"/>
         <v>48</v>
       </c>
-      <c r="H34" s="1" t="s">
+      <c r="H35" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I34" s="25">
-        <v>1</v>
-      </c>
-      <c r="J34" s="26">
+      <c r="I35" s="25">
+        <v>1</v>
+      </c>
+      <c r="J35" s="26">
         <v>3934</v>
       </c>
-      <c r="K34" s="26">
+      <c r="K35" s="26">
         <f t="shared" si="9"/>
         <v>3934</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B35" s="1" t="s">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B36" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C35" s="10">
+      <c r="C36" s="10">
         <v>42</v>
       </c>
-      <c r="D35" s="26">
+      <c r="D36" s="26">
         <v>13</v>
       </c>
-      <c r="E35" s="10">
+      <c r="E36" s="10">
         <f t="shared" si="8"/>
         <v>546</v>
       </c>
-      <c r="H35" s="1" t="s">
+      <c r="H36" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I35" s="25">
+      <c r="I36" s="25">
         <v>6</v>
       </c>
-      <c r="J35" s="26">
+      <c r="J36" s="26">
         <v>12</v>
       </c>
-      <c r="K35" s="26">
+      <c r="K36" s="26">
         <f t="shared" si="9"/>
         <v>72</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H36" s="1" t="s">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H37" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="I36" s="10">
+      <c r="I37" s="10">
         <v>63</v>
       </c>
-      <c r="J36" s="26">
+      <c r="J37" s="26">
         <v>13</v>
       </c>
-      <c r="K36" s="26">
+      <c r="K37" s="26">
         <f t="shared" si="9"/>
         <v>819</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B39" s="2">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" s="2">
         <v>4</v>
       </c>
-      <c r="C39" s="8"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="G39" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H39" s="2">
+      <c r="C40" s="8"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="G40" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H40" s="2">
         <v>5</v>
       </c>
-      <c r="I39" s="8"/>
-      <c r="J39" s="6"/>
-      <c r="K39" s="6"/>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B40" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D40" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E40" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I40" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="J40" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="K40" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="L40">
-        <v>13</v>
-      </c>
+      <c r="I40" s="8"/>
+      <c r="J40" s="6"/>
+      <c r="K40" s="6"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C41" s="5">
-        <v>4</v>
-      </c>
-      <c r="D41" s="10">
-        <v>450</v>
-      </c>
-      <c r="E41" s="10">
-        <f>D41*C41</f>
-        <v>1800</v>
+        <v>2</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>8</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I41" s="5">
-        <v>4</v>
-      </c>
-      <c r="J41" s="10">
-        <v>450</v>
-      </c>
-      <c r="K41" s="10">
-        <f>J41*I41</f>
-        <v>1800</v>
+        <v>2</v>
+      </c>
+      <c r="I41" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J41" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="K41" s="9" t="s">
+        <v>8</v>
       </c>
       <c r="L41">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C42" s="5">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D42" s="10">
-        <v>1699</v>
+        <v>450</v>
       </c>
       <c r="E42" s="10">
-        <f t="shared" ref="E42" si="10">D42*C42</f>
-        <v>15291</v>
+        <f>D42*C42</f>
+        <v>1800</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I42" s="5">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="J42" s="10">
-        <v>1699</v>
+        <v>450</v>
       </c>
       <c r="K42" s="10">
-        <f t="shared" ref="K42" si="11">J42*I42</f>
-        <v>11893</v>
+        <f>J42*I42</f>
+        <v>1800</v>
+      </c>
+      <c r="L42">
+        <v>12</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C43" s="5">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D43" s="10">
-        <v>1700</v>
+        <v>1699</v>
       </c>
       <c r="E43" s="10">
-        <f>D43*C43</f>
-        <v>1700</v>
+        <f t="shared" ref="E43" si="10">D43*C43</f>
+        <v>15291</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I43" s="5">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J43" s="10">
-        <v>1700</v>
+        <v>1699</v>
       </c>
       <c r="K43" s="10">
-        <f>J43*I43</f>
-        <v>1700</v>
+        <f t="shared" ref="K43" si="11">J43*I43</f>
+        <v>11893</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C44" s="5">
-        <f>2*C42+2*C43</f>
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D44" s="10">
-        <v>0.5</v>
+        <v>1700</v>
       </c>
       <c r="E44" s="10">
         <f>D44*C44</f>
-        <v>10</v>
+        <v>1700</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="I44" s="5">
-        <f>2*I42+2*I43</f>
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="J44" s="10">
-        <v>0.5</v>
+        <v>1700</v>
       </c>
       <c r="K44" s="10">
         <f>J44*I44</f>
-        <v>8</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C45" s="10"/>
+        <v>20</v>
+      </c>
+      <c r="C45" s="5">
+        <f>2*C43+2*C44</f>
+        <v>20</v>
+      </c>
       <c r="D45" s="10">
-        <v>0.85</v>
+        <v>0.5</v>
       </c>
       <c r="E45" s="10">
-        <f t="shared" ref="E45:E48" si="12">D45*C45</f>
-        <v>0</v>
+        <f>D45*C45</f>
+        <v>10</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I45" s="10"/>
+        <v>20</v>
+      </c>
+      <c r="I45" s="5">
+        <f>2*I43+2*I44</f>
+        <v>16</v>
+      </c>
       <c r="J45" s="10">
-        <v>0.85</v>
+        <v>0.5</v>
       </c>
       <c r="K45" s="10">
-        <f t="shared" ref="K45:K49" si="13">J45*I45</f>
-        <v>0</v>
+        <f>J45*I45</f>
+        <v>8</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C46" s="10"/>
+      <c r="D46" s="10">
+        <v>0.85</v>
+      </c>
+      <c r="E46" s="10">
+        <f t="shared" ref="E46:E49" si="12">D46*C46</f>
+        <v>0</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I46" s="10"/>
+      <c r="J46" s="10">
+        <v>0.85</v>
+      </c>
+      <c r="K46" s="10">
+        <f t="shared" ref="K46:K50" si="13">J46*I46</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B47" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C46" s="10">
-        <v>1</v>
-      </c>
-      <c r="D46" s="10">
+      <c r="C47" s="10">
+        <v>1</v>
+      </c>
+      <c r="D47" s="10">
         <v>1190</v>
       </c>
-      <c r="E46" s="10">
+      <c r="E47" s="10">
         <f t="shared" si="12"/>
         <v>1190</v>
       </c>
-      <c r="H46" s="1" t="s">
+      <c r="H47" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I46" s="10">
-        <v>1</v>
-      </c>
-      <c r="J46" s="10">
+      <c r="I47" s="10">
+        <v>1</v>
+      </c>
+      <c r="J47" s="10">
         <v>1190</v>
       </c>
-      <c r="K46" s="10">
+      <c r="K47" s="10">
         <f t="shared" si="13"/>
         <v>1190</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B47" s="1" t="s">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B48" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C47" s="25">
+      <c r="C48" s="25">
         <v>3</v>
       </c>
-      <c r="D47" s="26">
+      <c r="D48" s="26">
         <v>12</v>
       </c>
-      <c r="E47" s="26">
+      <c r="E48" s="26">
         <f t="shared" si="12"/>
         <v>36</v>
       </c>
-      <c r="H47" s="1" t="s">
+      <c r="H48" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I47" s="25">
-        <v>1</v>
-      </c>
-      <c r="J47" s="26">
+      <c r="I48" s="25">
+        <v>1</v>
+      </c>
+      <c r="J48" s="26">
         <v>3935</v>
       </c>
-      <c r="K47" s="26">
+      <c r="K48" s="26">
         <f t="shared" si="13"/>
         <v>3935</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B48" s="1" t="s">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B49" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C48" s="10">
+      <c r="C49" s="10">
         <v>27</v>
       </c>
-      <c r="D48" s="26">
+      <c r="D49" s="26">
         <v>13</v>
       </c>
-      <c r="E48" s="26">
+      <c r="E49" s="26">
         <f t="shared" si="12"/>
         <v>351</v>
       </c>
-      <c r="H48" s="1" t="s">
+      <c r="H49" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I48" s="25">
-        <v>2</v>
-      </c>
-      <c r="J48" s="26">
+      <c r="I49" s="25">
+        <v>2</v>
+      </c>
+      <c r="J49" s="26">
         <v>12</v>
       </c>
-      <c r="K48" s="26">
+      <c r="K49" s="26">
         <f t="shared" si="13"/>
         <v>24</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G49" s="12"/>
-      <c r="H49" s="1" t="s">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G50" s="12"/>
+      <c r="H50" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="I49" s="29">
+      <c r="I50" s="29">
         <v>21</v>
       </c>
-      <c r="J49" s="26">
+      <c r="J50" s="26">
         <v>13</v>
       </c>
-      <c r="K49" s="26">
+      <c r="K50" s="26">
         <f t="shared" si="13"/>
         <v>273</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G50" s="12"/>
-      <c r="H50" s="12"/>
-      <c r="I50" s="12"/>
-    </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B51" s="2" t="s">
+      <c r="G51" s="12"/>
+      <c r="H51" s="12"/>
+      <c r="I51" s="12"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C51" s="8"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="6"/>
-      <c r="H51" s="12"/>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B52" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C52" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D52" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E52" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="G52" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="H52" s="21"/>
-      <c r="L52">
-        <v>3</v>
-      </c>
+      <c r="C52" s="8"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+      <c r="H52" s="12"/>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B53" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C53" s="5">
-        <v>1</v>
-      </c>
-      <c r="D53" s="10">
-        <v>450</v>
-      </c>
-      <c r="E53" s="10">
-        <f>D53*C53</f>
-        <v>450</v>
-      </c>
-      <c r="H53" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I53" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C53" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="J53" s="9" t="s">
+      <c r="D53" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="K53" s="9" t="s">
+      <c r="E53" s="9" t="s">
         <v>8</v>
+      </c>
+      <c r="G53" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="H53" s="21"/>
+      <c r="L53">
+        <v>3</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B54" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C54" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D54" s="10">
-        <v>1699</v>
+        <v>450</v>
       </c>
       <c r="E54" s="10">
-        <f t="shared" ref="E54" si="14">D54*C54</f>
-        <v>3398</v>
-      </c>
-      <c r="H54" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="I54" s="10"/>
-      <c r="J54" s="10"/>
-      <c r="K54" s="10">
-        <f t="shared" ref="K54:K59" si="15">I54*J54</f>
-        <v>0</v>
+        <f>D54*C54</f>
+        <v>450</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I54" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J54" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="K54" s="9" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B55" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C55" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D55" s="10">
-        <v>1700</v>
+        <v>1699</v>
       </c>
       <c r="E55" s="10">
-        <f>D55*C55</f>
-        <v>1700</v>
+        <f t="shared" ref="E55" si="14">D55*C55</f>
+        <v>3398</v>
       </c>
       <c r="H55" s="19" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="I55" s="10"/>
       <c r="J55" s="10"/>
       <c r="K55" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="K55:K60" si="15">I55*J55</f>
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B56" s="1" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C56" s="5">
-        <f>2*C54+2*C55</f>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D56" s="10">
-        <v>0.5</v>
+        <v>1700</v>
       </c>
       <c r="E56" s="10">
         <f>D56*C56</f>
-        <v>3</v>
+        <v>1700</v>
       </c>
       <c r="H56" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="I56" s="10">
-        <v>1</v>
-      </c>
-      <c r="J56" s="10">
-        <v>20000</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="I56" s="10"/>
+      <c r="J56" s="10"/>
       <c r="K56" s="10">
         <f t="shared" si="15"/>
-        <v>20000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B57" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C57" s="10"/>
+        <v>20</v>
+      </c>
+      <c r="C57" s="5">
+        <f>2*C55+2*C56</f>
+        <v>6</v>
+      </c>
       <c r="D57" s="10">
-        <v>0.85</v>
+        <v>0.5</v>
       </c>
       <c r="E57" s="10">
-        <f t="shared" ref="E57:E61" si="16">D57*C57</f>
-        <v>0</v>
-      </c>
-      <c r="H57" s="28" t="s">
-        <v>35</v>
+        <f>D57*C57</f>
+        <v>3</v>
+      </c>
+      <c r="H57" s="19" t="s">
+        <v>31</v>
       </c>
       <c r="I57" s="10">
         <v>1</v>
       </c>
       <c r="J57" s="10">
-        <v>1400</v>
+        <v>20000</v>
       </c>
       <c r="K57" s="10">
         <f t="shared" si="15"/>
-        <v>1400</v>
+        <v>20000</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B58" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C58" s="10"/>
+      <c r="D58" s="10">
+        <v>0.85</v>
+      </c>
+      <c r="E58" s="10">
+        <f t="shared" ref="E58:E62" si="16">D58*C58</f>
+        <v>0</v>
+      </c>
+      <c r="H58" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="I58" s="10">
+        <v>1</v>
+      </c>
+      <c r="J58" s="10">
+        <v>1400</v>
+      </c>
+      <c r="K58" s="10">
+        <f t="shared" si="15"/>
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B59" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C58" s="10">
-        <v>1</v>
-      </c>
-      <c r="D58" s="10">
+      <c r="C59" s="10">
+        <v>1</v>
+      </c>
+      <c r="D59" s="10">
         <v>1190</v>
       </c>
-      <c r="E58" s="10">
+      <c r="E59" s="10">
         <f t="shared" si="16"/>
         <v>1190</v>
       </c>
-      <c r="H58" s="28" t="s">
+      <c r="H59" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="I58" s="10">
+      <c r="I59" s="10">
         <v>16</v>
       </c>
-      <c r="J58" s="10">
+      <c r="J59" s="10">
         <v>12</v>
       </c>
-      <c r="K58" s="10">
+      <c r="K59" s="10">
         <f t="shared" si="15"/>
         <v>192</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B59" s="1" t="s">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B60" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C59" s="25">
-        <v>1</v>
-      </c>
-      <c r="D59" s="26">
+      <c r="C60" s="25">
+        <v>1</v>
+      </c>
+      <c r="D60" s="26">
         <v>195</v>
       </c>
-      <c r="E59" s="26">
+      <c r="E60" s="26">
         <f t="shared" si="16"/>
         <v>195</v>
       </c>
-      <c r="H59" s="28" t="s">
+      <c r="H60" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="I59" s="10">
+      <c r="I60" s="10">
         <v>7</v>
       </c>
-      <c r="J59" s="26">
+      <c r="J60" s="26">
         <v>60</v>
       </c>
-      <c r="K59" s="10">
+      <c r="K60" s="10">
         <f t="shared" si="15"/>
         <v>420</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B60" s="1" t="s">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B61" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C60" s="25">
-        <v>1</v>
-      </c>
-      <c r="D60" s="26">
+      <c r="C61" s="25">
+        <v>1</v>
+      </c>
+      <c r="D61" s="26">
         <v>12</v>
       </c>
-      <c r="E60" s="26">
+      <c r="E61" s="26">
         <f t="shared" si="16"/>
         <v>12</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B61" s="1" t="s">
+    <row r="62" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B62" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C61" s="10">
+      <c r="C62" s="10">
         <v>6</v>
       </c>
-      <c r="D61" s="26">
+      <c r="D62" s="26">
         <v>13</v>
       </c>
-      <c r="E61" s="26">
+      <c r="E62" s="26">
         <f t="shared" si="16"/>
         <v>78</v>
       </c>
-      <c r="I61" s="18"/>
-      <c r="J61" s="18"/>
-      <c r="K61" s="18"/>
-    </row>
-    <row r="62" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D62" s="27"/>
       <c r="I62" s="18"/>
       <c r="J62" s="18"/>
       <c r="K62" s="18"/>
     </row>
     <row r="63" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="H63" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="I63" s="18">
-        <f>C61+I49+C48+I36+I20+C22+I9+C9</f>
-        <v>218</v>
-      </c>
+      <c r="D63" s="27"/>
+      <c r="I63" s="18"/>
       <c r="J63" s="18"/>
       <c r="K63" s="18"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="H64" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="I64" s="18">
+        <f>C62+I50+C49+I37+I20+C24+I9+C9</f>
+        <v>218</v>
+      </c>
+      <c r="J64" s="18"/>
+      <c r="K64" s="18"/>
+    </row>
+    <row r="65" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="H65" s="30" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="66" spans="6:9" x14ac:dyDescent="0.25">
-      <c r="F66" s="13" t="s">
+    <row r="67" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F67" s="13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="67" spans="6:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="F67" s="16"/>
-    </row>
-    <row r="68" spans="6:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F68" s="14" t="s">
+    <row r="68" spans="6:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="F68" s="16"/>
+    </row>
+    <row r="69" spans="6:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F69" s="14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="69" spans="6:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F69" s="15"/>
-    </row>
     <row r="70" spans="6:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F70" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="I70" s="18">
-        <v>400.15</v>
-      </c>
+      <c r="F70" s="15"/>
     </row>
     <row r="71" spans="6:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F71" s="17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I71" s="18">
-        <v>450.2</v>
+        <v>400.15</v>
       </c>
     </row>
     <row r="72" spans="6:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F72" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I72" s="18">
+        <v>450.2</v>
+      </c>
+    </row>
+    <row r="73" spans="6:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F73" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="I72" s="17">
+      <c r="I73" s="17">
         <v>620.29999999999995</v>
       </c>
-    </row>
-    <row r="73" spans="6:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F73" s="17"/>
     </row>
     <row r="74" spans="6:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F74" s="17"/>
     </row>
     <row r="75" spans="6:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F75" s="17" t="s">
+      <c r="F75" s="17"/>
+    </row>
+    <row r="76" spans="6:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F76" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="I75" s="20"/>
+      <c r="I76" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>